<commit_message>
Batch run for Iris 2nd round
</commit_message>
<xml_diff>
--- a/Data/Iris_inputs_v2.xlsx
+++ b/Data/Iris_inputs_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54E4875-E8CF-427B-B005-D8076DCE92CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB00D162-496C-4D37-A101-7EE879219508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1424,6 +1424,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1459,57 +1510,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1879,8 +1879,8 @@
   <dimension ref="A1:N120"/>
   <sheetViews>
     <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61:E64"/>
+      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1898,14 +1898,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="90" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="2" spans="1:9">
       <c r="B2" s="33"/>
@@ -1939,7 +1939,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="106" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1963,7 +1963,7 @@
       <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="90"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="I5" s="79"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="90"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
@@ -2014,7 +2014,7 @@
       <c r="I6" s="72"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="90"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="I7" s="72"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="90"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="90"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -2088,7 +2088,7 @@
       <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="90"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
@@ -2178,7 +2178,7 @@
       <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:9" s="35" customFormat="1" ht="14.7" customHeight="1">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="108" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -2206,7 +2206,7 @@
       <c r="I14" s="67"/>
     </row>
     <row r="15" spans="1:9" s="35" customFormat="1">
-      <c r="A15" s="92"/>
+      <c r="A15" s="109"/>
       <c r="B15" s="46" t="s">
         <v>74</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="I15" s="68"/>
     </row>
     <row r="16" spans="1:9" s="35" customFormat="1">
-      <c r="A16" s="92"/>
+      <c r="A16" s="109"/>
       <c r="B16" s="46" t="s">
         <v>75</v>
       </c>
@@ -2258,7 +2258,7 @@
       <c r="I16" s="68"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="110" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -2284,7 +2284,7 @@
       <c r="H17" s="85"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="93"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="25" t="s">
         <v>76</v>
       </c>
@@ -2308,7 +2308,7 @@
       <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="93"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="25" t="s">
         <v>79</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="H19" s="69"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="93"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="25" t="s">
         <v>80</v>
       </c>
@@ -2356,7 +2356,7 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="93"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="25" t="s">
         <v>86</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="93"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="25" t="s">
         <v>87</v>
       </c>
@@ -2404,7 +2404,7 @@
       <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="93"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="25" t="s">
         <v>90</v>
       </c>
@@ -2428,7 +2428,7 @@
       <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:13" ht="14.4" customHeight="1">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="111" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -2452,7 +2452,7 @@
       <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:13" ht="14.4" customHeight="1">
-      <c r="A25" s="95"/>
+      <c r="A25" s="112"/>
       <c r="B25" s="9" t="s">
         <v>12</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="95"/>
+      <c r="A26" s="112"/>
       <c r="B26" s="9" t="s">
         <v>13</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="95"/>
+      <c r="A27" s="112"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -2518,7 +2518,7 @@
       <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="95"/>
+      <c r="A28" s="112"/>
       <c r="B28" s="9" t="s">
         <v>14</v>
       </c>
@@ -2540,7 +2540,7 @@
       <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="95"/>
+      <c r="A29" s="112"/>
       <c r="B29" s="9" t="s">
         <v>15</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="95"/>
+      <c r="A30" s="112"/>
       <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="H30" s="49"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="95"/>
+      <c r="A31" s="112"/>
       <c r="B31" s="36" t="s">
         <v>17</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="95"/>
+      <c r="A32" s="112"/>
       <c r="B32" s="36" t="s">
         <v>18</v>
       </c>
@@ -2626,14 +2626,14 @@
         <v>114</v>
       </c>
       <c r="H32" s="50"/>
-      <c r="K32" s="99" t="s">
+      <c r="K32" s="87" t="s">
         <v>205</v>
       </c>
-      <c r="L32" s="100"/>
-      <c r="M32" s="101"/>
+      <c r="L32" s="88"/>
+      <c r="M32" s="89"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="95"/>
+      <c r="A33" s="112"/>
       <c r="B33" s="36" t="s">
         <v>22</v>
       </c>
@@ -2653,14 +2653,14 @@
         <v>115</v>
       </c>
       <c r="H33" s="80"/>
-      <c r="K33" s="110" t="s">
+      <c r="K33" s="98" t="s">
         <v>207</v>
       </c>
-      <c r="L33" s="112"/>
-      <c r="M33" s="111"/>
+      <c r="L33" s="100"/>
+      <c r="M33" s="99"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="95"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="36" t="s">
         <v>19</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="95"/>
+      <c r="A35" s="112"/>
       <c r="B35" s="36" t="s">
         <v>20</v>
       </c>
@@ -2723,7 +2723,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A36" s="107" t="s">
+      <c r="A36" s="95" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="51" t="s">
@@ -2749,14 +2749,14 @@
       </c>
       <c r="H36" s="82"/>
       <c r="I36" s="68"/>
-      <c r="K36" s="110" t="s">
+      <c r="K36" s="98" t="s">
         <v>206</v>
       </c>
-      <c r="L36" s="112"/>
-      <c r="M36" s="111"/>
+      <c r="L36" s="100"/>
+      <c r="M36" s="99"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="108"/>
+      <c r="A37" s="96"/>
       <c r="B37" s="51" t="s">
         <v>27</v>
       </c>
@@ -2791,7 +2791,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="108"/>
+      <c r="A38" s="96"/>
       <c r="B38" s="51" t="s">
         <v>28</v>
       </c>
@@ -2821,13 +2821,13 @@
       <c r="L38" s="49">
         <v>1500</v>
       </c>
-      <c r="M38" s="113">
+      <c r="M38" s="101">
         <f>L38*K38+K39*L39+K40*L40</f>
         <v>2805</v>
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="108"/>
+      <c r="A39" s="96"/>
       <c r="B39" s="51" t="s">
         <v>29</v>
       </c>
@@ -2857,10 +2857,10 @@
       <c r="L39" s="49">
         <v>6500</v>
       </c>
-      <c r="M39" s="114"/>
+      <c r="M39" s="102"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="109"/>
+      <c r="A40" s="97"/>
       <c r="B40" s="14" t="s">
         <v>165</v>
       </c>
@@ -2888,10 +2888,10 @@
       <c r="L40" s="49">
         <v>500</v>
       </c>
-      <c r="M40" s="115"/>
+      <c r="M40" s="103"/>
     </row>
     <row r="41" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A41" s="104" t="s">
+      <c r="A41" s="92" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="17" t="s">
@@ -2917,7 +2917,7 @@
       <c r="H41" s="49"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="105"/>
+      <c r="A42" s="93"/>
       <c r="B42" s="17" t="s">
         <v>33</v>
       </c>
@@ -2939,13 +2939,13 @@
         <v>123</v>
       </c>
       <c r="H42" s="49"/>
-      <c r="K42" s="110" t="s">
+      <c r="K42" s="98" t="s">
         <v>191</v>
       </c>
-      <c r="L42" s="111"/>
+      <c r="L42" s="99"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="105"/>
+      <c r="A43" s="93"/>
       <c r="B43" s="17" t="s">
         <v>34</v>
       </c>
@@ -2979,7 +2979,7 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="105"/>
+      <c r="A44" s="93"/>
       <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
@@ -3014,7 +3014,7 @@
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="105"/>
+      <c r="A45" s="93"/>
       <c r="B45" s="17" t="s">
         <v>36</v>
       </c>
@@ -3049,7 +3049,7 @@
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="105"/>
+      <c r="A46" s="93"/>
       <c r="B46" s="17" t="s">
         <v>37</v>
       </c>
@@ -3073,7 +3073,7 @@
       <c r="H46" s="49"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="106"/>
+      <c r="A47" s="94"/>
       <c r="B47" s="17" t="s">
         <v>151</v>
       </c>
@@ -3095,15 +3095,15 @@
         <v>162</v>
       </c>
       <c r="H47" s="49"/>
-      <c r="K47" s="110" t="s">
+      <c r="K47" s="98" t="s">
         <v>192</v>
       </c>
-      <c r="L47" s="112"/>
-      <c r="M47" s="112"/>
-      <c r="N47" s="111"/>
+      <c r="L47" s="100"/>
+      <c r="M47" s="100"/>
+      <c r="N47" s="99"/>
     </row>
     <row r="48" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A48" s="96" t="s">
+      <c r="A48" s="113" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="20" t="s">
@@ -3137,7 +3137,7 @@
       </c>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="97"/>
+      <c r="A49" s="114"/>
       <c r="B49" s="20" t="s">
         <v>171</v>
       </c>
@@ -3175,7 +3175,7 @@
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="97"/>
+      <c r="A50" s="114"/>
       <c r="B50" s="20" t="s">
         <v>173</v>
       </c>
@@ -3215,7 +3215,7 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="97"/>
+      <c r="A51" s="114"/>
       <c r="B51" s="20" t="s">
         <v>213</v>
       </c>
@@ -3245,7 +3245,7 @@
       <c r="N51" s="59"/>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="97"/>
+      <c r="A52" s="114"/>
       <c r="B52" s="20" t="s">
         <v>212</v>
       </c>
@@ -3285,7 +3285,7 @@
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="97"/>
+      <c r="A53" s="114"/>
       <c r="B53" s="20" t="s">
         <v>217</v>
       </c>
@@ -3325,7 +3325,7 @@
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="97"/>
+      <c r="A54" s="114"/>
       <c r="B54" s="20" t="s">
         <v>170</v>
       </c>
@@ -3350,7 +3350,7 @@
       <c r="I54" s="71"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="97"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="20" t="s">
         <v>174</v>
       </c>
@@ -3384,7 +3384,7 @@
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="97"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="23" t="s">
         <v>208</v>
       </c>
@@ -3419,7 +3419,7 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="97"/>
+      <c r="A57" s="114"/>
       <c r="B57" s="23" t="s">
         <v>209</v>
       </c>
@@ -3453,7 +3453,7 @@
       </c>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="97"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="23" t="s">
         <v>163</v>
       </c>
@@ -3486,7 +3486,7 @@
       </c>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="97"/>
+      <c r="A59" s="114"/>
       <c r="B59" s="23" t="s">
         <v>164</v>
       </c>
@@ -3509,7 +3509,7 @@
       <c r="H59" s="49"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="97"/>
+      <c r="A60" s="114"/>
       <c r="B60" s="23" t="s">
         <v>221</v>
       </c>
@@ -3531,7 +3531,7 @@
       <c r="H60" s="73"/>
     </row>
     <row r="61" spans="1:14" ht="14.4" customHeight="1">
-      <c r="A61" s="97"/>
+      <c r="A61" s="114"/>
       <c r="B61" s="41" t="s">
         <v>41</v>
       </c>
@@ -3563,7 +3563,7 @@
       </c>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="97"/>
+      <c r="A62" s="114"/>
       <c r="B62" s="41" t="s">
         <v>42</v>
       </c>
@@ -3595,7 +3595,7 @@
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="97"/>
+      <c r="A63" s="114"/>
       <c r="B63" s="41" t="s">
         <v>92</v>
       </c>
@@ -3627,7 +3627,7 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="98"/>
+      <c r="A64" s="115"/>
       <c r="B64" s="41" t="s">
         <v>93</v>
       </c>
@@ -3659,7 +3659,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" ht="14.4" customHeight="1">
-      <c r="A65" s="87" t="s">
+      <c r="A65" s="104" t="s">
         <v>49</v>
       </c>
       <c r="B65" s="55" t="s">
@@ -3683,7 +3683,7 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="88"/>
+      <c r="A66" s="105"/>
       <c r="B66" s="55" t="s">
         <v>59</v>
       </c>
@@ -3705,7 +3705,7 @@
       <c r="H66" s="84"/>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="88"/>
+      <c r="A67" s="105"/>
       <c r="B67" s="55" t="s">
         <v>51</v>
       </c>
@@ -3727,7 +3727,7 @@
       <c r="H67" s="84"/>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="88"/>
+      <c r="A68" s="105"/>
       <c r="B68" s="55" t="s">
         <v>52</v>
       </c>
@@ -3749,7 +3749,7 @@
       <c r="H68" s="84"/>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="88"/>
+      <c r="A69" s="105"/>
       <c r="B69" s="55" t="s">
         <v>53</v>
       </c>
@@ -3771,7 +3771,7 @@
       <c r="H69" s="84"/>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="88"/>
+      <c r="A70" s="105"/>
       <c r="B70" s="55" t="s">
         <v>94</v>
       </c>
@@ -3793,7 +3793,7 @@
       <c r="H70" s="84"/>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="88"/>
+      <c r="A71" s="105"/>
       <c r="B71" s="55" t="s">
         <v>54</v>
       </c>
@@ -3816,7 +3816,7 @@
       <c r="K71" s="13"/>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="88"/>
+      <c r="A72" s="105"/>
       <c r="B72" s="55" t="s">
         <v>60</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="88"/>
+      <c r="A73" s="105"/>
       <c r="B73" s="55" t="s">
         <v>55</v>
       </c>
@@ -3862,7 +3862,7 @@
       <c r="K73" s="13"/>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="88"/>
+      <c r="A74" s="105"/>
       <c r="B74" s="55" t="s">
         <v>56</v>
       </c>
@@ -3885,7 +3885,7 @@
       <c r="K74" s="13"/>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="88"/>
+      <c r="A75" s="105"/>
       <c r="B75" s="55" t="s">
         <v>57</v>
       </c>
@@ -3908,7 +3908,7 @@
       <c r="K75" s="13"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="88"/>
+      <c r="A76" s="105"/>
       <c r="B76" s="55" t="s">
         <v>96</v>
       </c>
@@ -3931,7 +3931,7 @@
       <c r="K76" s="13"/>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="88"/>
+      <c r="A77" s="105"/>
       <c r="B77" s="55" t="s">
         <v>58</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="H77" s="84"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="88"/>
+      <c r="A78" s="105"/>
       <c r="B78" s="55" t="s">
         <v>61</v>
       </c>
@@ -3975,7 +3975,7 @@
       <c r="H78" s="84"/>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="88"/>
+      <c r="A79" s="105"/>
       <c r="B79" s="55" t="s">
         <v>62</v>
       </c>
@@ -3997,7 +3997,7 @@
       <c r="H79" s="84"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="88"/>
+      <c r="A80" s="105"/>
       <c r="B80" s="55" t="s">
         <v>63</v>
       </c>
@@ -4019,7 +4019,7 @@
       <c r="H80" s="84"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="88"/>
+      <c r="A81" s="105"/>
       <c r="B81" s="55" t="s">
         <v>64</v>
       </c>
@@ -4041,7 +4041,7 @@
       <c r="H81" s="84"/>
     </row>
     <row r="82" spans="1:11">
-      <c r="A82" s="88"/>
+      <c r="A82" s="105"/>
       <c r="B82" s="55" t="s">
         <v>95</v>
       </c>
@@ -4112,6 +4112,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A65:A82"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A24:A35"/>
+    <mergeCell ref="A48:A64"/>
     <mergeCell ref="K32:M32"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A41:A47"/>
@@ -4121,12 +4127,6 @@
     <mergeCell ref="M38:M40"/>
     <mergeCell ref="K33:M33"/>
     <mergeCell ref="K36:M36"/>
-    <mergeCell ref="A65:A82"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="A24:A35"/>
-    <mergeCell ref="A48:A64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4138,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22540C2-7758-43CC-8CAC-337C735D93EA}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="104" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E64" sqref="C61:E64"/>
+    <sheetView topLeftCell="A38" zoomScale="104" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4153,14 +4153,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="90" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="4" t="s">
@@ -4186,7 +4186,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="106" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -4210,7 +4210,7 @@
       <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="90"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4234,7 +4234,7 @@
       <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="90"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="90"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
@@ -4284,7 +4284,7 @@
       <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="90"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="90"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -4332,21 +4332,20 @@
       <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="90"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="44">
-        <f>747-Iris_original!C10</f>
-        <v>326</v>
+        <v>421</v>
       </c>
       <c r="D10" s="31">
         <f t="shared" si="0"/>
-        <v>293.40000000000003</v>
+        <v>378.90000000000003</v>
       </c>
       <c r="E10" s="31">
         <f t="shared" si="1"/>
-        <v>358.6</v>
+        <v>463.1</v>
       </c>
       <c r="F10" s="45" t="s">
         <v>6</v>
@@ -4423,7 +4422,7 @@
       <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="108" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -4450,7 +4449,7 @@
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="92"/>
+      <c r="A15" s="109"/>
       <c r="B15" s="46" t="s">
         <v>74</v>
       </c>
@@ -4475,7 +4474,7 @@
       <c r="H15" s="83"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="92"/>
+      <c r="A16" s="109"/>
       <c r="B16" s="46" t="s">
         <v>75</v>
       </c>
@@ -4500,7 +4499,7 @@
       <c r="H16" s="84"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="110" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -4526,7 +4525,7 @@
       <c r="H17" s="85"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="93"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="25" t="s">
         <v>76</v>
       </c>
@@ -4550,7 +4549,7 @@
       <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="93"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="25" t="s">
         <v>79</v>
       </c>
@@ -4574,7 +4573,7 @@
       <c r="H19" s="69"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="93"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="25" t="s">
         <v>80</v>
       </c>
@@ -4598,7 +4597,7 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="93"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="25" t="s">
         <v>86</v>
       </c>
@@ -4622,7 +4621,7 @@
       <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="93"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="25" t="s">
         <v>87</v>
       </c>
@@ -4646,7 +4645,7 @@
       <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="93"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="25" t="s">
         <v>90</v>
       </c>
@@ -4670,7 +4669,7 @@
       <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="111" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -4694,7 +4693,7 @@
       <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="95"/>
+      <c r="A25" s="112"/>
       <c r="B25" s="9" t="s">
         <v>12</v>
       </c>
@@ -4716,7 +4715,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="95"/>
+      <c r="A26" s="112"/>
       <c r="B26" s="9" t="s">
         <v>13</v>
       </c>
@@ -4738,7 +4737,7 @@
       <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="95"/>
+      <c r="A27" s="112"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -4760,7 +4759,7 @@
       <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="95"/>
+      <c r="A28" s="112"/>
       <c r="B28" s="9" t="s">
         <v>14</v>
       </c>
@@ -4782,7 +4781,7 @@
       <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="95"/>
+      <c r="A29" s="112"/>
       <c r="B29" s="9" t="s">
         <v>15</v>
       </c>
@@ -4804,7 +4803,7 @@
       <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="95"/>
+      <c r="A30" s="112"/>
       <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
@@ -4826,7 +4825,7 @@
       <c r="H30" s="49"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="95"/>
+      <c r="A31" s="112"/>
       <c r="B31" s="36" t="s">
         <v>17</v>
       </c>
@@ -4848,7 +4847,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="95"/>
+      <c r="A32" s="112"/>
       <c r="B32" s="36" t="s">
         <v>18</v>
       </c>
@@ -4870,7 +4869,7 @@
       <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="95"/>
+      <c r="A33" s="112"/>
       <c r="B33" s="36" t="s">
         <v>22</v>
       </c>
@@ -4892,7 +4891,7 @@
       <c r="H33" s="80"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="95"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="36" t="s">
         <v>19</v>
       </c>
@@ -4914,7 +4913,7 @@
       <c r="H34" s="81"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="95"/>
+      <c r="A35" s="112"/>
       <c r="B35" s="36" t="s">
         <v>20</v>
       </c>
@@ -4936,7 +4935,7 @@
       <c r="H35" s="81"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="107" t="s">
+      <c r="A36" s="95" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="51" t="s">
@@ -4963,7 +4962,7 @@
       <c r="H36" s="82"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="108"/>
+      <c r="A37" s="96"/>
       <c r="B37" s="51" t="s">
         <v>27</v>
       </c>
@@ -4988,7 +4987,7 @@
       <c r="H37" s="80"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="108"/>
+      <c r="A38" s="96"/>
       <c r="B38" s="51" t="s">
         <v>28</v>
       </c>
@@ -5013,7 +5012,7 @@
       <c r="H38" s="81"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="108"/>
+      <c r="A39" s="96"/>
       <c r="B39" s="51" t="s">
         <v>29</v>
       </c>
@@ -5038,7 +5037,7 @@
       <c r="H39" s="81"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="109"/>
+      <c r="A40" s="97"/>
       <c r="B40" s="14" t="s">
         <v>165</v>
       </c>
@@ -5062,7 +5061,7 @@
       <c r="H40" s="82"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="104" t="s">
+      <c r="A41" s="92" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="17" t="s">
@@ -5088,7 +5087,7 @@
       <c r="H41" s="49"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="105"/>
+      <c r="A42" s="93"/>
       <c r="B42" s="17" t="s">
         <v>33</v>
       </c>
@@ -5112,7 +5111,7 @@
       <c r="H42" s="49"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="105"/>
+      <c r="A43" s="93"/>
       <c r="B43" s="17" t="s">
         <v>34</v>
       </c>
@@ -5136,7 +5135,7 @@
       <c r="H43" s="49"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="105"/>
+      <c r="A44" s="93"/>
       <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
@@ -5160,7 +5159,7 @@
       <c r="H44" s="49"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="105"/>
+      <c r="A45" s="93"/>
       <c r="B45" s="17" t="s">
         <v>36</v>
       </c>
@@ -5184,7 +5183,7 @@
       <c r="H45" s="49"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="105"/>
+      <c r="A46" s="93"/>
       <c r="B46" s="17" t="s">
         <v>37</v>
       </c>
@@ -5208,7 +5207,7 @@
       <c r="H46" s="49"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="106"/>
+      <c r="A47" s="94"/>
       <c r="B47" s="17" t="s">
         <v>151</v>
       </c>
@@ -5232,7 +5231,7 @@
       <c r="H47" s="49"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="96" t="s">
+      <c r="A48" s="113" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="20" t="s">
@@ -5259,7 +5258,7 @@
       <c r="H48" s="49"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="97"/>
+      <c r="A49" s="114"/>
       <c r="B49" s="20" t="s">
         <v>171</v>
       </c>
@@ -5284,7 +5283,7 @@
       <c r="H49" s="80"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="97"/>
+      <c r="A50" s="114"/>
       <c r="B50" s="20" t="s">
         <v>173</v>
       </c>
@@ -5309,7 +5308,7 @@
       <c r="H50" s="81"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="97"/>
+      <c r="A51" s="114"/>
       <c r="B51" s="20" t="s">
         <v>213</v>
       </c>
@@ -5334,7 +5333,7 @@
       <c r="H51" s="81"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="97"/>
+      <c r="A52" s="114"/>
       <c r="B52" s="20" t="s">
         <v>212</v>
       </c>
@@ -5359,7 +5358,7 @@
       <c r="H52" s="81"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="97"/>
+      <c r="A53" s="114"/>
       <c r="B53" s="20" t="s">
         <v>217</v>
       </c>
@@ -5384,7 +5383,7 @@
       <c r="H53" s="81"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="97"/>
+      <c r="A54" s="114"/>
       <c r="B54" s="20" t="s">
         <v>170</v>
       </c>
@@ -5408,7 +5407,7 @@
       <c r="H54" s="81"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="97"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="20" t="s">
         <v>174</v>
       </c>
@@ -5432,7 +5431,7 @@
       <c r="H55" s="81"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="97"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="23" t="s">
         <v>208</v>
       </c>
@@ -5457,7 +5456,7 @@
       <c r="H56" s="81"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="97"/>
+      <c r="A57" s="114"/>
       <c r="B57" s="23" t="s">
         <v>209</v>
       </c>
@@ -5481,7 +5480,7 @@
       <c r="H57" s="81"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="97"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="23" t="s">
         <v>163</v>
       </c>
@@ -5506,7 +5505,7 @@
       <c r="H58" s="82"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="97"/>
+      <c r="A59" s="114"/>
       <c r="B59" s="23" t="s">
         <v>164</v>
       </c>
@@ -5529,7 +5528,7 @@
       <c r="H59" s="49"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="97"/>
+      <c r="A60" s="114"/>
       <c r="B60" s="23" t="s">
         <v>221</v>
       </c>
@@ -5551,7 +5550,7 @@
       <c r="H60" s="73"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="97"/>
+      <c r="A61" s="114"/>
       <c r="B61" s="41" t="s">
         <v>41</v>
       </c>
@@ -5573,7 +5572,7 @@
       <c r="H61" s="80"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="97"/>
+      <c r="A62" s="114"/>
       <c r="B62" s="41" t="s">
         <v>42</v>
       </c>
@@ -5595,7 +5594,7 @@
       <c r="H62" s="81"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="97"/>
+      <c r="A63" s="114"/>
       <c r="B63" s="41" t="s">
         <v>92</v>
       </c>
@@ -5617,7 +5616,7 @@
       <c r="H63" s="81"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="98"/>
+      <c r="A64" s="115"/>
       <c r="B64" s="41" t="s">
         <v>93</v>
       </c>
@@ -5639,7 +5638,7 @@
       <c r="H64" s="82"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="87" t="s">
+      <c r="A65" s="104" t="s">
         <v>49</v>
       </c>
       <c r="B65" s="55" t="s">
@@ -5663,7 +5662,7 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="88"/>
+      <c r="A66" s="105"/>
       <c r="B66" s="55" t="s">
         <v>59</v>
       </c>
@@ -5685,7 +5684,7 @@
       <c r="H66" s="84"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="88"/>
+      <c r="A67" s="105"/>
       <c r="B67" s="55" t="s">
         <v>51</v>
       </c>
@@ -5707,7 +5706,7 @@
       <c r="H67" s="84"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="88"/>
+      <c r="A68" s="105"/>
       <c r="B68" s="55" t="s">
         <v>52</v>
       </c>
@@ -5729,7 +5728,7 @@
       <c r="H68" s="84"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="88"/>
+      <c r="A69" s="105"/>
       <c r="B69" s="55" t="s">
         <v>53</v>
       </c>
@@ -5751,7 +5750,7 @@
       <c r="H69" s="84"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="88"/>
+      <c r="A70" s="105"/>
       <c r="B70" s="55" t="s">
         <v>94</v>
       </c>
@@ -5773,7 +5772,7 @@
       <c r="H70" s="84"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="88"/>
+      <c r="A71" s="105"/>
       <c r="B71" s="55" t="s">
         <v>54</v>
       </c>
@@ -5795,7 +5794,7 @@
       <c r="H71" s="84"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="88"/>
+      <c r="A72" s="105"/>
       <c r="B72" s="55" t="s">
         <v>60</v>
       </c>
@@ -5817,7 +5816,7 @@
       <c r="H72" s="84"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="88"/>
+      <c r="A73" s="105"/>
       <c r="B73" s="55" t="s">
         <v>55</v>
       </c>
@@ -5839,7 +5838,7 @@
       <c r="H73" s="84"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="88"/>
+      <c r="A74" s="105"/>
       <c r="B74" s="55" t="s">
         <v>56</v>
       </c>
@@ -5861,7 +5860,7 @@
       <c r="H74" s="84"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="88"/>
+      <c r="A75" s="105"/>
       <c r="B75" s="55" t="s">
         <v>57</v>
       </c>
@@ -5883,7 +5882,7 @@
       <c r="H75" s="84"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="88"/>
+      <c r="A76" s="105"/>
       <c r="B76" s="55" t="s">
         <v>96</v>
       </c>
@@ -5905,7 +5904,7 @@
       <c r="H76" s="84"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="88"/>
+      <c r="A77" s="105"/>
       <c r="B77" s="55" t="s">
         <v>58</v>
       </c>
@@ -5927,7 +5926,7 @@
       <c r="H77" s="84"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="88"/>
+      <c r="A78" s="105"/>
       <c r="B78" s="55" t="s">
         <v>61</v>
       </c>
@@ -5949,7 +5948,7 @@
       <c r="H78" s="84"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="88"/>
+      <c r="A79" s="105"/>
       <c r="B79" s="55" t="s">
         <v>62</v>
       </c>
@@ -5971,7 +5970,7 @@
       <c r="H79" s="84"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="88"/>
+      <c r="A80" s="105"/>
       <c r="B80" s="55" t="s">
         <v>63</v>
       </c>
@@ -5993,7 +5992,7 @@
       <c r="H80" s="84"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="88"/>
+      <c r="A81" s="105"/>
       <c r="B81" s="55" t="s">
         <v>64</v>
       </c>
@@ -6015,7 +6014,7 @@
       <c r="H81" s="84"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="88"/>
+      <c r="A82" s="105"/>
       <c r="B82" s="55" t="s">
         <v>95</v>
       </c>
@@ -6058,8 +6057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FDFB89-F078-4F84-A115-0B27F39D5164}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6073,14 +6072,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="90" t="s">
         <v>224</v>
       </c>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" s="33"/>
@@ -6114,7 +6113,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="106" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -6138,7 +6137,7 @@
       <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="90"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
@@ -6162,7 +6161,7 @@
       <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="90"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
@@ -6187,7 +6186,7 @@
       <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="90"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
@@ -6212,7 +6211,7 @@
       <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="90"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="8" t="s">
         <v>154</v>
       </c>
@@ -6236,7 +6235,7 @@
       <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="90"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="8" t="s">
         <v>65</v>
       </c>
@@ -6260,20 +6259,20 @@
       <c r="H9" s="54"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="90"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="44">
-        <v>747</v>
+        <v>421</v>
       </c>
       <c r="D10" s="31">
         <f t="shared" si="0"/>
-        <v>672.30000000000007</v>
+        <v>378.90000000000003</v>
       </c>
       <c r="E10" s="31">
         <f t="shared" si="1"/>
-        <v>821.7</v>
+        <v>463.1</v>
       </c>
       <c r="F10" s="45" t="s">
         <v>6</v>
@@ -6350,7 +6349,7 @@
       <c r="H13" s="86"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="108" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="46" t="s">
@@ -6377,7 +6376,7 @@
       <c r="H14" s="66"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="92"/>
+      <c r="A15" s="109"/>
       <c r="B15" s="46" t="s">
         <v>74</v>
       </c>
@@ -6402,7 +6401,7 @@
       <c r="H15" s="83"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="92"/>
+      <c r="A16" s="109"/>
       <c r="B16" s="46" t="s">
         <v>75</v>
       </c>
@@ -6427,7 +6426,7 @@
       <c r="H16" s="84"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="110" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -6453,7 +6452,7 @@
       <c r="H17" s="85"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="93"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="25" t="s">
         <v>76</v>
       </c>
@@ -6477,7 +6476,7 @@
       <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="93"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="25" t="s">
         <v>79</v>
       </c>
@@ -6501,7 +6500,7 @@
       <c r="H19" s="69"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="93"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="25" t="s">
         <v>80</v>
       </c>
@@ -6525,7 +6524,7 @@
       <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="93"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="25" t="s">
         <v>86</v>
       </c>
@@ -6549,7 +6548,7 @@
       <c r="H21" s="49"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="93"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="25" t="s">
         <v>87</v>
       </c>
@@ -6573,7 +6572,7 @@
       <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="93"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="25" t="s">
         <v>90</v>
       </c>
@@ -6597,7 +6596,7 @@
       <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="111" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -6621,7 +6620,7 @@
       <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="95"/>
+      <c r="A25" s="112"/>
       <c r="B25" s="9" t="s">
         <v>12</v>
       </c>
@@ -6643,7 +6642,7 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="95"/>
+      <c r="A26" s="112"/>
       <c r="B26" s="9" t="s">
         <v>13</v>
       </c>
@@ -6665,7 +6664,7 @@
       <c r="H26" s="49"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="95"/>
+      <c r="A27" s="112"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
@@ -6687,7 +6686,7 @@
       <c r="H27" s="49"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="95"/>
+      <c r="A28" s="112"/>
       <c r="B28" s="9" t="s">
         <v>14</v>
       </c>
@@ -6709,7 +6708,7 @@
       <c r="H28" s="49"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="95"/>
+      <c r="A29" s="112"/>
       <c r="B29" s="9" t="s">
         <v>15</v>
       </c>
@@ -6731,7 +6730,7 @@
       <c r="H29" s="49"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="95"/>
+      <c r="A30" s="112"/>
       <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
@@ -6753,7 +6752,7 @@
       <c r="H30" s="49"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="95"/>
+      <c r="A31" s="112"/>
       <c r="B31" s="36" t="s">
         <v>17</v>
       </c>
@@ -6775,7 +6774,7 @@
       <c r="H31" s="50"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="95"/>
+      <c r="A32" s="112"/>
       <c r="B32" s="36" t="s">
         <v>18</v>
       </c>
@@ -6797,7 +6796,7 @@
       <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="95"/>
+      <c r="A33" s="112"/>
       <c r="B33" s="36" t="s">
         <v>22</v>
       </c>
@@ -6819,7 +6818,7 @@
       <c r="H33" s="80"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="95"/>
+      <c r="A34" s="112"/>
       <c r="B34" s="36" t="s">
         <v>19</v>
       </c>
@@ -6841,7 +6840,7 @@
       <c r="H34" s="81"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="95"/>
+      <c r="A35" s="112"/>
       <c r="B35" s="36" t="s">
         <v>20</v>
       </c>
@@ -6863,7 +6862,7 @@
       <c r="H35" s="81"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="107" t="s">
+      <c r="A36" s="95" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="51" t="s">
@@ -6890,7 +6889,7 @@
       <c r="H36" s="82"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="108"/>
+      <c r="A37" s="96"/>
       <c r="B37" s="51" t="s">
         <v>27</v>
       </c>
@@ -6915,7 +6914,7 @@
       <c r="H37" s="80"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="108"/>
+      <c r="A38" s="96"/>
       <c r="B38" s="51" t="s">
         <v>28</v>
       </c>
@@ -6940,7 +6939,7 @@
       <c r="H38" s="81"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="108"/>
+      <c r="A39" s="96"/>
       <c r="B39" s="51" t="s">
         <v>29</v>
       </c>
@@ -6965,7 +6964,7 @@
       <c r="H39" s="81"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="109"/>
+      <c r="A40" s="97"/>
       <c r="B40" s="14" t="s">
         <v>165</v>
       </c>
@@ -6989,7 +6988,7 @@
       <c r="H40" s="82"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="104" t="s">
+      <c r="A41" s="92" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="17" t="s">
@@ -7015,7 +7014,7 @@
       <c r="H41" s="49"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="105"/>
+      <c r="A42" s="93"/>
       <c r="B42" s="17" t="s">
         <v>33</v>
       </c>
@@ -7039,7 +7038,7 @@
       <c r="H42" s="49"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="105"/>
+      <c r="A43" s="93"/>
       <c r="B43" s="17" t="s">
         <v>34</v>
       </c>
@@ -7063,7 +7062,7 @@
       <c r="H43" s="49"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="105"/>
+      <c r="A44" s="93"/>
       <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
@@ -7087,7 +7086,7 @@
       <c r="H44" s="49"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="105"/>
+      <c r="A45" s="93"/>
       <c r="B45" s="17" t="s">
         <v>36</v>
       </c>
@@ -7111,7 +7110,7 @@
       <c r="H45" s="49"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="105"/>
+      <c r="A46" s="93"/>
       <c r="B46" s="17" t="s">
         <v>37</v>
       </c>
@@ -7135,7 +7134,7 @@
       <c r="H46" s="49"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="106"/>
+      <c r="A47" s="94"/>
       <c r="B47" s="17" t="s">
         <v>151</v>
       </c>
@@ -7159,7 +7158,7 @@
       <c r="H47" s="49"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="96" t="s">
+      <c r="A48" s="113" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="20" t="s">
@@ -7186,7 +7185,7 @@
       <c r="H48" s="49"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="97"/>
+      <c r="A49" s="114"/>
       <c r="B49" s="20" t="s">
         <v>171</v>
       </c>
@@ -7211,7 +7210,7 @@
       <c r="H49" s="80"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="97"/>
+      <c r="A50" s="114"/>
       <c r="B50" s="20" t="s">
         <v>173</v>
       </c>
@@ -7236,7 +7235,7 @@
       <c r="H50" s="81"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="97"/>
+      <c r="A51" s="114"/>
       <c r="B51" s="20" t="s">
         <v>213</v>
       </c>
@@ -7261,7 +7260,7 @@
       <c r="H51" s="81"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="97"/>
+      <c r="A52" s="114"/>
       <c r="B52" s="20" t="s">
         <v>212</v>
       </c>
@@ -7286,7 +7285,7 @@
       <c r="H52" s="81"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="97"/>
+      <c r="A53" s="114"/>
       <c r="B53" s="20" t="s">
         <v>217</v>
       </c>
@@ -7311,7 +7310,7 @@
       <c r="H53" s="81"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="97"/>
+      <c r="A54" s="114"/>
       <c r="B54" s="20" t="s">
         <v>170</v>
       </c>
@@ -7335,7 +7334,7 @@
       <c r="H54" s="81"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="97"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="20" t="s">
         <v>174</v>
       </c>
@@ -7359,7 +7358,7 @@
       <c r="H55" s="81"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="97"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="23" t="s">
         <v>208</v>
       </c>
@@ -7384,7 +7383,7 @@
       <c r="H56" s="81"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="97"/>
+      <c r="A57" s="114"/>
       <c r="B57" s="23" t="s">
         <v>209</v>
       </c>
@@ -7408,7 +7407,7 @@
       <c r="H57" s="81"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="97"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="23" t="s">
         <v>163</v>
       </c>
@@ -7433,7 +7432,7 @@
       <c r="H58" s="82"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="97"/>
+      <c r="A59" s="114"/>
       <c r="B59" s="23" t="s">
         <v>164</v>
       </c>
@@ -7456,7 +7455,7 @@
       <c r="H59" s="49"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="97"/>
+      <c r="A60" s="114"/>
       <c r="B60" s="23" t="s">
         <v>221</v>
       </c>
@@ -7478,7 +7477,7 @@
       <c r="H60" s="73"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="97"/>
+      <c r="A61" s="114"/>
       <c r="B61" s="41" t="s">
         <v>41</v>
       </c>
@@ -7500,7 +7499,7 @@
       <c r="H61" s="80"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="97"/>
+      <c r="A62" s="114"/>
       <c r="B62" s="41" t="s">
         <v>42</v>
       </c>
@@ -7522,7 +7521,7 @@
       <c r="H62" s="81"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="97"/>
+      <c r="A63" s="114"/>
       <c r="B63" s="41" t="s">
         <v>92</v>
       </c>
@@ -7544,7 +7543,7 @@
       <c r="H63" s="81"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="98"/>
+      <c r="A64" s="115"/>
       <c r="B64" s="41" t="s">
         <v>93</v>
       </c>
@@ -7566,7 +7565,7 @@
       <c r="H64" s="82"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="87" t="s">
+      <c r="A65" s="104" t="s">
         <v>49</v>
       </c>
       <c r="B65" s="55" t="s">
@@ -7590,7 +7589,7 @@
       <c r="H65" s="83"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="88"/>
+      <c r="A66" s="105"/>
       <c r="B66" s="55" t="s">
         <v>59</v>
       </c>
@@ -7612,7 +7611,7 @@
       <c r="H66" s="84"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="88"/>
+      <c r="A67" s="105"/>
       <c r="B67" s="55" t="s">
         <v>51</v>
       </c>
@@ -7634,7 +7633,7 @@
       <c r="H67" s="84"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="88"/>
+      <c r="A68" s="105"/>
       <c r="B68" s="55" t="s">
         <v>52</v>
       </c>
@@ -7656,7 +7655,7 @@
       <c r="H68" s="84"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="88"/>
+      <c r="A69" s="105"/>
       <c r="B69" s="55" t="s">
         <v>53</v>
       </c>
@@ -7678,7 +7677,7 @@
       <c r="H69" s="84"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="88"/>
+      <c r="A70" s="105"/>
       <c r="B70" s="55" t="s">
         <v>94</v>
       </c>
@@ -7700,7 +7699,7 @@
       <c r="H70" s="84"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="88"/>
+      <c r="A71" s="105"/>
       <c r="B71" s="55" t="s">
         <v>54</v>
       </c>
@@ -7722,7 +7721,7 @@
       <c r="H71" s="84"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="88"/>
+      <c r="A72" s="105"/>
       <c r="B72" s="55" t="s">
         <v>60</v>
       </c>
@@ -7744,7 +7743,7 @@
       <c r="H72" s="84"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="88"/>
+      <c r="A73" s="105"/>
       <c r="B73" s="55" t="s">
         <v>55</v>
       </c>
@@ -7766,7 +7765,7 @@
       <c r="H73" s="84"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="88"/>
+      <c r="A74" s="105"/>
       <c r="B74" s="55" t="s">
         <v>56</v>
       </c>
@@ -7788,7 +7787,7 @@
       <c r="H74" s="84"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="88"/>
+      <c r="A75" s="105"/>
       <c r="B75" s="55" t="s">
         <v>57</v>
       </c>
@@ -7810,7 +7809,7 @@
       <c r="H75" s="84"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="88"/>
+      <c r="A76" s="105"/>
       <c r="B76" s="55" t="s">
         <v>96</v>
       </c>
@@ -7832,7 +7831,7 @@
       <c r="H76" s="84"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="88"/>
+      <c r="A77" s="105"/>
       <c r="B77" s="55" t="s">
         <v>58</v>
       </c>
@@ -7854,7 +7853,7 @@
       <c r="H77" s="84"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="88"/>
+      <c r="A78" s="105"/>
       <c r="B78" s="55" t="s">
         <v>61</v>
       </c>
@@ -7876,7 +7875,7 @@
       <c r="H78" s="84"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="88"/>
+      <c r="A79" s="105"/>
       <c r="B79" s="55" t="s">
         <v>62</v>
       </c>
@@ -7898,7 +7897,7 @@
       <c r="H79" s="84"/>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="88"/>
+      <c r="A80" s="105"/>
       <c r="B80" s="55" t="s">
         <v>63</v>
       </c>
@@ -7920,7 +7919,7 @@
       <c r="H80" s="84"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="88"/>
+      <c r="A81" s="105"/>
       <c r="B81" s="55" t="s">
         <v>64</v>
       </c>
@@ -7942,7 +7941,7 @@
       <c r="H81" s="84"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="88"/>
+      <c r="A82" s="105"/>
       <c r="B82" s="55" t="s">
         <v>95</v>
       </c>
@@ -7989,6 +7988,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D2CC3865CED4124A9830BAAA78333A39" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="74fbc97153726fbf9f4b2acfe0ba4f2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="47151ffa-27c1-491d-bdc5-fff6d8a44614" xmlns:ns4="2a729546-cf4e-435c-aabc-21366d2421e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef40a5df47e7cf58b55af26490b848e0" ns3:_="" ns4:_="">
     <xsd:import namespace="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
@@ -8211,36 +8225,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D48284-4FE0-49DC-82DA-D80B72208958}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9031FEDD-5FF8-4C9C-AF51-AEFA4BF396D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
-    <ds:schemaRef ds:uri="2a729546-cf4e-435c-aabc-21366d2421e1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8263,9 +8251,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9031FEDD-5FF8-4C9C-AF51-AEFA4BF396D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D48284-4FE0-49DC-82DA-D80B72208958}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="47151ffa-27c1-491d-bdc5-fff6d8a44614"/>
+    <ds:schemaRef ds:uri="2a729546-cf4e-435c-aabc-21366d2421e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>